<commit_message>
changed grid definition so that it is directly used in base node / storage node / connection node names.
</commit_message>
<xml_diff>
--- a/example_data/nodes/nodes.xlsx
+++ b/example_data/nodes/nodes.xlsx
@@ -52,7 +52,7 @@
     <t xml:space="preserve">balance_type_none</t>
   </si>
   <si>
-    <t xml:space="preserve">dheat</t>
+    <t xml:space="preserve">heat</t>
   </si>
   <si>
     <t xml:space="preserve">ts:heat1</t>
@@ -404,7 +404,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
added co2 node into example data. adjusted default_candi_units.
</commit_message>
<xml_diff>
--- a/example_data/nodes/nodes.xlsx
+++ b/example_data/nodes/nodes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t xml:space="preserve">node</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">ts:heat1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">co2</t>
   </si>
 </sst>
 </file>
@@ -96,7 +99,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,6 +128,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF972F"/>
         <bgColor rgb="FFFF8080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF666666"/>
+        <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
   </fills>
@@ -169,7 +178,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -215,6 +224,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -275,7 +288,7 @@
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF972F"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF666666"/>
       <rgbColor rgb="FF77BC65"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
@@ -401,10 +414,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -497,6 +510,15 @@
         <v>10</v>
       </c>
     </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="D7" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
added output recipe for co2 emissions.
</commit_message>
<xml_diff>
--- a/example_data/nodes/nodes.xlsx
+++ b/example_data/nodes/nodes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t xml:space="preserve">node</t>
   </si>
@@ -417,7 +417,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -515,6 +515,9 @@
         <v>12</v>
       </c>
       <c r="B7" s="12"/>
+      <c r="C7" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="D7" s="9" t="s">
         <v>9</v>
       </c>

</xml_diff>